<commit_message>
Updated Basepage nad LoginPage for automation with DUO, Scenario 1 and Scenario 5 ,Scenario 2 needs date format update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NEU Semesters\Fall2025_Semester_4\INFO_6255_Software_Quality_Control\Assignment\Selenium\INFO6255-Selenium-Assignment\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66BC1E5-B41E-4A2A-832E-73A236E07114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F79FB2-019F-4383-A365-FA93A52C84D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6E96723E-205B-41E5-9136-C14533771537}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Follow-Up</t>
+  </si>
+  <si>
+    <t>raut.ni@northeastern.edu</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,9 +487,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C81E029F-9050-48BB-918E-3BAB766A0092}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -490,7 +507,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +562,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>45986</v>

</xml_diff>